<commit_message>
IV curve analysis and organisation
</commit_message>
<xml_diff>
--- a/WO3196_dev2_IV_curves.xlsx
+++ b/WO3196_dev2_IV_curves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rijk\Documents\MEP\MEP_control_software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9A3036D-36F3-442C-B921-0645BD0A22B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D931D4D8-0FB1-4CF3-A53C-F4A37E429866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-5040" windowWidth="29040" windowHeight="15840" xr2:uid="{4E66C9AB-82E7-483C-A789-CD534FE62061}"/>
+    <workbookView xWindow="28680" yWindow="-3735" windowWidth="19440" windowHeight="15000" xr2:uid="{4E66C9AB-82E7-483C-A789-CD534FE62061}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="39">
   <si>
     <t>Resistances IV curve light</t>
   </si>
@@ -99,6 +99,57 @@
   </si>
   <si>
     <t>0127_1854_WO3196_full_IV_curve_h2_100nA</t>
+  </si>
+  <si>
+    <t>2point and 4point measurements</t>
+  </si>
+  <si>
+    <t>0220_1422_WO3196_iv_65C_4point</t>
+  </si>
+  <si>
+    <t>4 point air</t>
+  </si>
+  <si>
+    <t>2 point air</t>
+  </si>
+  <si>
+    <t>0220_1449_WO3196_iv_65C_2point</t>
+  </si>
+  <si>
+    <t>0220_1518_WO3196_iv_65C_h2_4point</t>
+  </si>
+  <si>
+    <t>4 point h2</t>
+  </si>
+  <si>
+    <t>0220_1530_WO3196_iv_65C_h2_2point</t>
+  </si>
+  <si>
+    <t>2 point h2</t>
+  </si>
+  <si>
+    <t>Difference between contact resistance in H2 and in Air</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>4point</t>
+  </si>
+  <si>
+    <t>2point</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Contact std</t>
   </si>
 </sst>
 </file>
@@ -157,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -166,11 +217,177 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -359,6 +576,53 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -373,15 +637,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02ADF916-690F-4E74-8E52-45BFA2C9747A}" name="Table2" displayName="Table2" ref="A2:F22" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A2:F22" xr:uid="{C669BD6D-AEC3-4C27-8AD6-33044C59E370}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02ADF916-690F-4E74-8E52-45BFA2C9747A}" name="Table2" displayName="Table2" ref="A2:F22" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A2:F22" xr:uid="{C669BD6D-AEC3-4C27-8AD6-33044C59E370}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Plus"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="All"/>
+        <filter val="Middle"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{57E615B1-1E1E-444E-8C68-838A942E9C18}" name="Name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8596E6C0-5DAA-4B91-B679-983DAC2B3C53}" name="Measurement" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{74D0E527-5423-4BE6-949E-9DE3A7C2C639}" name="Direction" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{33D0CEF0-15BB-4B63-9222-AD215A4CE249}" name="Position" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{32C0EF77-2D41-4819-A561-4D9FE1728DAF}" name="R (Ohm)" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{86FDCB3C-116C-4F70-A406-863ACBE0C7BD}" name="R Std (Ohm)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{57E615B1-1E1E-444E-8C68-838A942E9C18}" name="Name" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{8596E6C0-5DAA-4B91-B679-983DAC2B3C53}" name="Measurement" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{74D0E527-5423-4BE6-949E-9DE3A7C2C639}" name="Direction" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{33D0CEF0-15BB-4B63-9222-AD215A4CE249}" name="Position" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{32C0EF77-2D41-4819-A561-4D9FE1728DAF}" name="R (Ohm)" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{86FDCB3C-116C-4F70-A406-863ACBE0C7BD}" name="R Std (Ohm)" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D3D27DE8-4822-4C9E-AF9E-71465279D840}" name="Table22" displayName="Table22" ref="A25:F41" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A25:F41" xr:uid="{6D0BDC06-6FBE-4071-8B51-45C32536D851}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8494BB97-A4B0-4C9A-9A1C-DBB91294A4F1}" name="Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6583055A-42A8-4671-A685-4C7D41C01609}" name="Measurement" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{C0BFC36E-D2CC-4784-9833-A400F66F35F2}" name="Direction" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{944E5C3F-4F53-4BD5-8606-CE021E8A0D15}" name="Position" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{DFCB8247-0007-4DC7-BC0E-6918B61A0916}" name="R (Ohm)" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D5C80107-7799-47B2-88C0-9B2D392466AC}" name="R Std (Ohm)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{69F006CD-1778-4749-97BE-767BE561B92B}" name="Table3" displayName="Table3" ref="A44:E46" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A44:E46" xr:uid="{853C54D8-0076-47EB-8F6B-28F164054773}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F4B9FEAC-4B12-473A-AB08-35CE8BBA5B34}" name="Gas"/>
+    <tableColumn id="2" xr3:uid="{DABF68AC-EF86-4B0C-87E3-77FD3734C127}" name="4point"/>
+    <tableColumn id="3" xr3:uid="{7134B1FC-7AEB-44A2-8793-D72B87874A17}" name="2point"/>
+    <tableColumn id="4" xr3:uid="{52F81127-7AEF-4DF7-92B2-60153B4C2C65}" name="Contact"/>
+    <tableColumn id="5" xr3:uid="{C3AF4012-CACD-44C8-8285-083BF373FB84}" name="Contact std"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -684,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8E1A5E1-40A1-4E37-9E82-F79302CE3204}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="A1:F22"/>
+      <selection activeCell="A2" sqref="A2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +1052,7 @@
         <v>19904.700644799999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -767,7 +1072,7 @@
         <v>152734.148863284</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -787,7 +1092,7 @@
         <v>109358.879405841</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -807,7 +1112,7 @@
         <v>43149.817957918</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -827,7 +1132,7 @@
         <v>147706.139370327</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -867,7 +1172,7 @@
         <v>74166.683974225904</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -887,7 +1192,7 @@
         <v>35782.047570575101</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -907,7 +1212,7 @@
         <v>33143.080502166304</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -927,7 +1232,7 @@
         <v>27834.462731885102</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -947,7 +1252,7 @@
         <v>81130.296231860993</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -987,7 +1292,7 @@
         <v>14668.4108616866</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1007,7 +1312,7 @@
         <v>8734.3304880966407</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1047,7 +1352,7 @@
         <v>288524.40633688797</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -1067,7 +1372,7 @@
         <v>752009.05828439805</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
@@ -1087,7 +1392,7 @@
         <v>419242.18916454603</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1412,7 @@
         <v>264903.880877516</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1136,7 +1441,9 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -1144,34 +1451,431 @@
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="A25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="A26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3">
+        <v>57662467.307866603</v>
+      </c>
+      <c r="F26" s="3">
+        <v>536594.44611825806</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="A27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="5">
+        <v>24769844.365186099</v>
+      </c>
+      <c r="F27" s="5">
+        <v>70480.355317855196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5">
+        <v>54345843.0624891</v>
+      </c>
+      <c r="F28" s="5">
+        <v>861051.35324881098</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="5">
+        <v>60203084.383946002</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1210411.5483027601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="5">
+        <v>24391470.934402</v>
+      </c>
+      <c r="F30" s="5">
+        <v>48395.771238795904</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5">
+        <v>53215474.404310197</v>
+      </c>
+      <c r="F31" s="5">
+        <v>2179104.64897023</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="5">
+        <v>163783226.457607</v>
+      </c>
+      <c r="F32" s="5">
+        <v>523837.46905012801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="5">
+        <v>166721117.63563201</v>
+      </c>
+      <c r="F33" s="5">
+        <v>449074.30707394402</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="5">
+        <v>63481425.448886096</v>
+      </c>
+      <c r="F34" s="5">
+        <v>378402.54198409902</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="5">
+        <v>23903970.365336701</v>
+      </c>
+      <c r="F35" s="5">
+        <v>26057.830860440499</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="5">
+        <v>64089375.399888702</v>
+      </c>
+      <c r="F36" s="5">
+        <v>271529.56080825097</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="5">
+        <v>64964485.008407302</v>
+      </c>
+      <c r="F37" s="5">
+        <v>610092.06684011105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="5">
+        <v>23742255.423094399</v>
+      </c>
+      <c r="F38" s="7">
+        <v>7437.9907061061704</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="5">
+        <v>62764554.5378718</v>
+      </c>
+      <c r="F39" s="5">
+        <v>491143.037693955</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="5">
+        <v>194282861.593353</v>
+      </c>
+      <c r="F40" s="5">
+        <v>221588.549311982</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="5">
+        <v>194717747.40534401</v>
+      </c>
+      <c r="F41" s="5">
+        <v>188880.668954244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="5">
+        <f>AVERAGE(E27,E30)</f>
+        <v>24580657.64979405</v>
+      </c>
+      <c r="C45" s="5">
+        <f>AVERAGE(E32:E33)</f>
+        <v>165252172.0466195</v>
+      </c>
+      <c r="D45" s="5">
+        <f>(Table3[[#This Row],[2point]]-Table3[[#This Row],[4point]])/2</f>
+        <v>70335757.198412731</v>
+      </c>
+      <c r="E45" s="5">
+        <f>MAX(F27,F30,F32:F33)</f>
+        <v>523837.46905012801</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="8">
+        <f>AVERAGE(E35,E38)</f>
+        <v>23823112.89421555</v>
+      </c>
+      <c r="C46" s="8">
+        <f>AVERAGE(E40:E41)</f>
+        <v>194500304.49934852</v>
+      </c>
+      <c r="D46" s="5">
+        <f>(Table3[[#This Row],[2point]]-Table3[[#This Row],[4point]])/2</f>
+        <v>85338595.802566484</v>
+      </c>
+      <c r="E46" s="8">
+        <f>MAX(F35,F38,F40:F41)</f>
+        <v>221588.549311982</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>